<commit_message>
Funktion zum automatischen Schildern von Sonderzielen hinzugefügt
- Beim Erreichen der letzten Haltestelle, wird automatisch "Fahrtende" geschildert
- Beim aktivieren der Pause-Funktion wird automatisch "Pause" geschlidert".
genaures siehe Readme.

fixes #5
</commit_message>
<xml_diff>
--- a/Dokumentation.xlsx
+++ b/Dokumentation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58332FC8-A128-4CAE-A8DA-85BD32E0D4E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86FFC61-7137-48E8-BD99-2B64BBA4E1EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="404">
   <si>
     <t>Name</t>
   </si>
@@ -1232,6 +1232,36 @@
   </si>
   <si>
     <t>Bestätigt die nächste Fahrt und schaltet in den Pause-Modus</t>
+  </si>
+  <si>
+    <t>Schildert automatisch auf "Fahrtende", sobald die letzte Haltestelle erreicht wird</t>
+  </si>
+  <si>
+    <t>nuntius_printer_autoSetTripEndTerminus</t>
+  </si>
+  <si>
+    <t>nuntius_printer_option_terminusCodeTripEnd</t>
+  </si>
+  <si>
+    <t>nuntius_printer_option_terminusCodeBreak</t>
+  </si>
+  <si>
+    <t>Terminus-Code, der für das "Pause"-Ziel verwendet werden soll</t>
+  </si>
+  <si>
+    <t>Terminus-Code, der für das "Fahrtende"-Ziel verwendet werden soll</t>
+  </si>
+  <si>
+    <t>nuntius_printer_loadOptions</t>
+  </si>
+  <si>
+    <t>lädt beim Start die Optionen aus der Hofdatei</t>
+  </si>
+  <si>
+    <t>nuntius_printer_hasHofFileOptions</t>
+  </si>
+  <si>
+    <t>Existieren Hofdatei-spezifische Optionen?</t>
   </si>
 </sst>
 </file>
@@ -1525,15 +1555,15 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="99.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1914,369 +1944,393 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
+      <c r="A52" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B54" s="3" t="s">
+      <c r="B56" s="6"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="3" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>116</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>117</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>118</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>372</v>
+        <v>131</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>373</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>383</v>
+        <v>132</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>385</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>133</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>372</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>383</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>384</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="6" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B77" s="6"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B78" s="3" t="s">
+      <c r="B80" s="6"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>134</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>135</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>136</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B83" s="6"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>213</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>214</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>226</v>
+        <v>136</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>215</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>175</v>
-      </c>
+      <c r="A86" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B86" s="6"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>228</v>
+        <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>186</v>
+        <v>231</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>187</v>
+        <v>233</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
+        <v>222</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>223</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>224</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>387</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B102" s="5" t="s">
         <v>388</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A86:B86"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A80:B80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2604,10 +2658,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717CEF75-956F-4D6D-ADE3-21264BBAF87D}">
-  <dimension ref="A1:K78"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2737,21 +2791,18 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>400</v>
       </c>
       <c r="B11" t="s">
-        <v>311</v>
-      </c>
-      <c r="C11" t="s">
-        <v>304</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C12" t="s">
         <v>304</v>
@@ -2759,10 +2810,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>379</v>
+        <v>248</v>
       </c>
       <c r="B13" t="s">
-        <v>380</v>
+        <v>312</v>
       </c>
       <c r="C13" t="s">
         <v>304</v>
@@ -2770,10 +2821,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>249</v>
+        <v>379</v>
       </c>
       <c r="B14" t="s">
-        <v>313</v>
+        <v>380</v>
       </c>
       <c r="C14" t="s">
         <v>304</v>
@@ -2781,10 +2832,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>250</v>
+        <v>395</v>
       </c>
       <c r="B15" t="s">
-        <v>314</v>
+        <v>394</v>
       </c>
       <c r="C15" t="s">
         <v>304</v>
@@ -2792,537 +2843,553 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>249</v>
       </c>
       <c r="B16" t="s">
-        <v>315</v>
-      </c>
-      <c r="D16" t="s">
-        <v>316</v>
+        <v>313</v>
+      </c>
+      <c r="C16" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s">
-        <v>317</v>
+        <v>314</v>
+      </c>
+      <c r="C17" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>318</v>
+        <v>315</v>
+      </c>
+      <c r="D18" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>251</v>
       </c>
       <c r="B19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>252</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>322</v>
-      </c>
-      <c r="D22" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>253</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B24" t="s">
-        <v>324</v>
+        <v>322</v>
+      </c>
+      <c r="D24" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>381</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s">
-        <v>391</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>389</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s">
-        <v>392</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="B29" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="B30" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>257</v>
+        <v>390</v>
       </c>
       <c r="B31" t="s">
-        <v>328</v>
+        <v>393</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>258</v>
+        <v>381</v>
       </c>
       <c r="B32" t="s">
-        <v>329</v>
+        <v>382</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B33" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>258</v>
       </c>
       <c r="B34" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B35" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>261</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
-        <v>333</v>
-      </c>
-      <c r="D36" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B37" t="s">
-        <v>335</v>
-      </c>
-      <c r="D37" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B38" t="s">
-        <v>337</v>
+        <v>333</v>
+      </c>
+      <c r="D38" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B39" t="s">
-        <v>338</v>
+        <v>335</v>
+      </c>
+      <c r="D39" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B40" t="s">
-        <v>339</v>
-      </c>
-      <c r="C40" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B41" t="s">
-        <v>340</v>
-      </c>
-      <c r="D41" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>369</v>
+        <v>265</v>
       </c>
       <c r="B42" t="s">
-        <v>370</v>
-      </c>
-      <c r="D42" t="s">
-        <v>371</v>
+        <v>339</v>
+      </c>
+      <c r="C42" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B43" t="s">
-        <v>342</v>
+        <v>340</v>
+      </c>
+      <c r="D43" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>268</v>
+        <v>369</v>
       </c>
       <c r="B44" t="s">
-        <v>343</v>
-      </c>
-      <c r="C44" t="s">
-        <v>304</v>
+        <v>370</v>
+      </c>
+      <c r="D44" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B45" t="s">
-        <v>345</v>
-      </c>
-      <c r="D45" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>366</v>
+        <v>268</v>
       </c>
       <c r="B46" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B47" t="s">
-        <v>344</v>
-      </c>
-      <c r="C47" t="s">
-        <v>304</v>
+        <v>345</v>
+      </c>
+      <c r="D47" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>271</v>
+        <v>366</v>
       </c>
       <c r="B48" t="s">
-        <v>347</v>
-      </c>
-      <c r="D48" t="s">
-        <v>346</v>
+        <v>365</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>367</v>
+        <v>270</v>
       </c>
       <c r="B49" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B50" t="s">
-        <v>348</v>
+        <v>347</v>
+      </c>
+      <c r="D50" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>274</v>
+        <v>367</v>
       </c>
       <c r="B51" t="s">
-        <v>349</v>
-      </c>
-      <c r="D51" t="s">
-        <v>350</v>
+        <v>368</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B52" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B53" t="s">
-        <v>352</v>
+        <v>349</v>
+      </c>
+      <c r="D53" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B54" t="s">
-        <v>353</v>
-      </c>
-      <c r="D54" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B55" t="s">
-        <v>355</v>
-      </c>
-      <c r="C55" t="s">
-        <v>304</v>
+        <v>352</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B56" t="s">
-        <v>356</v>
+        <v>353</v>
+      </c>
+      <c r="D56" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B57" t="s">
-        <v>357</v>
-      </c>
-      <c r="D57" t="s">
-        <v>358</v>
+        <v>355</v>
+      </c>
+      <c r="C57" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B58" t="s">
-        <v>359</v>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>279</v>
+      </c>
+      <c r="B59" t="s">
+        <v>357</v>
+      </c>
+      <c r="D59" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B60" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>282</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>283</v>
-      </c>
-      <c r="B62" s="7"/>
-      <c r="D62" s="7"/>
+        <v>281</v>
+      </c>
+      <c r="B62" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>284</v>
-      </c>
-      <c r="B63" s="7"/>
-      <c r="D63" s="7"/>
+        <v>282</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B64" s="7"/>
       <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B65" s="7"/>
       <c r="D65" s="7"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B66" s="7"/>
       <c r="D66" s="7"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B67" s="7"/>
       <c r="D67" s="7"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B68" s="7"/>
       <c r="D68" s="7"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B69" s="7"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B70" s="7"/>
       <c r="D70" s="7"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B71" s="7"/>
       <c r="D71" s="7"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B72" s="7"/>
       <c r="D72" s="7"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B73" s="7"/>
       <c r="D73" s="7"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B74" s="7"/>
       <c r="D74" s="7"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B75" s="7"/>
       <c r="D75" s="7"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B76" s="7"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>298</v>
-      </c>
-      <c r="B77" t="s">
-        <v>363</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="B77" s="7"/>
+      <c r="D77" s="7"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>297</v>
+      </c>
+      <c r="B78" s="7"/>
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>298</v>
+      </c>
+      <c r="B79" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>299</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B80" t="s">
         <v>364</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B61:B76"/>
-    <mergeCell ref="D61:D76"/>
+    <mergeCell ref="B63:B78"/>
+    <mergeCell ref="D63:D78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
removed debug reset button
</commit_message>
<xml_diff>
--- a/Dokumentation.xlsx
+++ b/Dokumentation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8D2834-55C2-410C-83BE-B338F655009A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D1D043-2175-4308-A026-64679B4FF7F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variablen" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="420">
   <si>
     <t>Name</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>nuntius_printer_input2</t>
-  </si>
-  <si>
-    <t>[Dient zu debug-Zwecken] - Testbutton neben dem Drucker zum vollständigen Zurücksetzen/Neustarten</t>
   </si>
   <si>
     <t>Wenn die neben dem Drucker liegende (inaktive) Fahrerkarten angeklickt (aufgelegt) wird</t>
@@ -1392,9 +1389,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1403,6 +1397,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1641,49 +1638,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="10"/>
+      <c r="A6" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1691,762 +1688,762 @@
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="B13" s="10"/>
+      <c r="A13" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B20" s="10"/>
+      <c r="A20" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="B27" s="10"/>
+      <c r="A27" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" s="9"/>
     </row>
     <row r="28" spans="1:2" ht="297" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>402</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="99" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="66" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>376</v>
-      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
-        <v>413</v>
+      <c r="A58" s="8" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>400</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>396</v>
-      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B63" s="10"/>
+      <c r="A63" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B63" s="9"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>371</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B87" s="10"/>
+      <c r="A87" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B87" s="9"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B93" s="10"/>
+      <c r="A93" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B93" s="9"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>385</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="B111" s="5" t="s">
         <v>404</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B112" s="5" t="s">
         <v>414</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -2469,10 +2466,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2488,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
@@ -2496,7 +2493,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -2504,7 +2501,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>42</v>
@@ -2512,7 +2509,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
@@ -2520,7 +2517,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
@@ -2528,7 +2525,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
@@ -2536,7 +2533,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -2544,7 +2541,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>47</v>
@@ -2552,7 +2549,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>48</v>
@@ -2560,7 +2557,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>49</v>
@@ -2568,7 +2565,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
       </c>
       <c r="C11" t="s">
         <v>50</v>
@@ -2576,56 +2576,53 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>60</v>
@@ -2633,15 +2630,15 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>63</v>
@@ -2649,7 +2646,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
         <v>64</v>
@@ -2657,23 +2654,23 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
         <v>66</v>
@@ -2681,31 +2678,34 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
       </c>
       <c r="C27" t="s">
         <v>70</v>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>77</v>
@@ -2724,7 +2724,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
         <v>78</v>
@@ -2735,10 +2735,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
         <v>73</v>
@@ -2746,7 +2743,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
         <v>74</v>
@@ -2754,7 +2751,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
         <v>75</v>
@@ -2762,19 +2759,11 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>40</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="B33" s="2"/>
       <c r="C33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
         <v>373</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" t="s">
-        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -2787,8 +2776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717CEF75-956F-4D6D-ADE3-21264BBAF87D}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62:B80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2808,7 +2797,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -2837,157 +2826,157 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>397</v>
+      </c>
+      <c r="B11" t="s">
         <v>398</v>
-      </c>
-      <c r="B11" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>377</v>
+      </c>
+      <c r="B14" t="s">
         <v>378</v>
       </c>
-      <c r="B14" t="s">
-        <v>379</v>
-      </c>
       <c r="C14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2995,18 +2984,18 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
+        <v>313</v>
+      </c>
+      <c r="D18" t="s">
         <v>314</v>
-      </c>
-      <c r="D18" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -3014,7 +3003,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -3022,7 +3011,7 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -3030,7 +3019,7 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -3038,477 +3027,477 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B24" t="s">
+        <v>320</v>
+      </c>
+      <c r="D24" t="s">
         <v>321</v>
-      </c>
-      <c r="D24" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B33" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B34" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B36" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B37" t="s">
+        <v>331</v>
+      </c>
+      <c r="D37" t="s">
         <v>332</v>
-      </c>
-      <c r="D37" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B38" t="s">
+        <v>333</v>
+      </c>
+      <c r="D38" t="s">
         <v>334</v>
-      </c>
-      <c r="D38" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B42" t="s">
+        <v>338</v>
+      </c>
+      <c r="D42" t="s">
         <v>339</v>
-      </c>
-      <c r="D42" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>367</v>
+      </c>
+      <c r="B43" t="s">
         <v>368</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>369</v>
-      </c>
-      <c r="D43" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B44" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B45" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B46" t="s">
+        <v>343</v>
+      </c>
+      <c r="D46" t="s">
         <v>344</v>
-      </c>
-      <c r="D46" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B47" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B49" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D49" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>365</v>
+      </c>
+      <c r="B50" t="s">
         <v>366</v>
-      </c>
-      <c r="B50" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B51" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B52" t="s">
+        <v>347</v>
+      </c>
+      <c r="D52" t="s">
         <v>348</v>
-      </c>
-      <c r="D52" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B53" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B54" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B55" t="s">
+        <v>351</v>
+      </c>
+      <c r="D55" t="s">
         <v>352</v>
-      </c>
-      <c r="D55" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B56" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C56" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B57" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B58" t="s">
+        <v>355</v>
+      </c>
+      <c r="D58" t="s">
         <v>356</v>
-      </c>
-      <c r="D58" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B59" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B61" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>281</v>
-      </c>
-      <c r="B62" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="D62" s="10" t="s">
         <v>360</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>282</v>
-      </c>
-      <c r="B63" s="7"/>
-      <c r="D63" s="7"/>
+        <v>281</v>
+      </c>
+      <c r="B63" s="10"/>
+      <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>283</v>
-      </c>
-      <c r="B64" s="7"/>
-      <c r="D64" s="7"/>
+        <v>282</v>
+      </c>
+      <c r="B64" s="10"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>284</v>
-      </c>
-      <c r="B65" s="7"/>
-      <c r="D65" s="7"/>
+        <v>283</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="D65" s="10"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>285</v>
-      </c>
-      <c r="B66" s="7"/>
-      <c r="D66" s="7"/>
+        <v>284</v>
+      </c>
+      <c r="B66" s="10"/>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>286</v>
-      </c>
-      <c r="B67" s="7"/>
-      <c r="D67" s="7"/>
+        <v>285</v>
+      </c>
+      <c r="B67" s="10"/>
+      <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>287</v>
-      </c>
-      <c r="B68" s="7"/>
-      <c r="D68" s="7"/>
+        <v>286</v>
+      </c>
+      <c r="B68" s="10"/>
+      <c r="D68" s="10"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>288</v>
-      </c>
-      <c r="B69" s="7"/>
-      <c r="D69" s="7"/>
+        <v>287</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="D69" s="10"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>289</v>
-      </c>
-      <c r="B70" s="7"/>
-      <c r="D70" s="7"/>
+        <v>288</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="D70" s="10"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>290</v>
-      </c>
-      <c r="B71" s="7"/>
-      <c r="D71" s="7"/>
+        <v>289</v>
+      </c>
+      <c r="B71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>291</v>
-      </c>
-      <c r="B72" s="7"/>
-      <c r="D72" s="7"/>
+        <v>290</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="D72" s="10"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>292</v>
-      </c>
-      <c r="B73" s="7"/>
-      <c r="D73" s="7"/>
+        <v>291</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>293</v>
-      </c>
-      <c r="B74" s="7"/>
-      <c r="D74" s="7"/>
+        <v>292</v>
+      </c>
+      <c r="B74" s="10"/>
+      <c r="D74" s="10"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>294</v>
-      </c>
-      <c r="B75" s="7"/>
-      <c r="D75" s="7"/>
+        <v>293</v>
+      </c>
+      <c r="B75" s="10"/>
+      <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>295</v>
-      </c>
-      <c r="B76" s="7"/>
-      <c r="D76" s="7"/>
+        <v>294</v>
+      </c>
+      <c r="B76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>296</v>
-      </c>
-      <c r="B77" s="7"/>
-      <c r="D77" s="7"/>
+        <v>295</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="D77" s="10"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>418</v>
-      </c>
-      <c r="B78" s="7"/>
-      <c r="D78" s="7"/>
+        <v>417</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="D78" s="10"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>419</v>
-      </c>
-      <c r="B79" s="7"/>
-      <c r="D79" s="7"/>
+        <v>418</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="D79" s="10"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>420</v>
-      </c>
-      <c r="B80" s="7"/>
-      <c r="D80" s="7"/>
+        <v>419</v>
+      </c>
+      <c r="B80" s="10"/>
+      <c r="D80" s="10"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B81" s="6"/>
@@ -3516,18 +3505,18 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B82" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B83" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ladezeit beim Einlesen der Fahrerkarte
</commit_message>
<xml_diff>
--- a/Dokumentation.xlsx
+++ b/Dokumentation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C7948D-C147-4174-925D-2BD46F6A681E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E9BA63-8698-4BBC-948A-A38E6B6A3155}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variablen" sheetId="2" r:id="rId1"/>
@@ -1757,6 +1757,45 @@
     <t>Ziel-Page nach Ablauf der Wartezeit</t>
   </si>
   <si>
+    <t>nuntius_printer_visLoadingInfo</t>
+  </si>
+  <si>
+    <t>Informationstext auf dem Ladebildschrim</t>
+  </si>
+  <si>
+    <t>nuntius_printer_ui_loadingInfo</t>
+  </si>
+  <si>
+    <t>Lade- und Fehlermeldungsinfotext</t>
+  </si>
+  <si>
+    <t>nuntius_printer_updateWaitTimer</t>
+  </si>
+  <si>
+    <t>Aktualisiert den Wartezeit-Timer für die Simulation von Ladezeiten</t>
+  </si>
+  <si>
+    <t>nuntius_printer_startWaitTime</t>
+  </si>
+  <si>
+    <t>nuntius_printer_goToPageAfterWaitTime</t>
+  </si>
+  <si>
+    <t>Öffnet die "Bitte Warten"-Seite für die Ladezeit-Simulation</t>
+  </si>
+  <si>
+    <t>Wartezeit in Sekunden</t>
+  </si>
+  <si>
+    <t>Wait-Reason für die Ladezeit</t>
+  </si>
+  <si>
+    <t>Zielseite nach Ablauf der Wartezeit</t>
+  </si>
+  <si>
+    <t>Startet die Wartezeit mit dem gegebenen Wartegrund</t>
+  </si>
+  <si>
     <t>Enum-Wert für den Grund der Wartezeit, die gestartet wurde.
 -1 = undefiniert
 0 = Fahrerkarte einlesen
@@ -1766,46 +1805,8 @@
 4 = Ziel prüfen
 5 = Warten auf Ticketdruck
 6 = Pause aktivieren
-7 = Abmelden</t>
-  </si>
-  <si>
-    <t>nuntius_printer_visLoadingInfo</t>
-  </si>
-  <si>
-    <t>Informationstext auf dem Ladebildschrim</t>
-  </si>
-  <si>
-    <t>nuntius_printer_ui_loadingInfo</t>
-  </si>
-  <si>
-    <t>Lade- und Fehlermeldungsinfotext</t>
-  </si>
-  <si>
-    <t>nuntius_printer_updateWaitTimer</t>
-  </si>
-  <si>
-    <t>Aktualisiert den Wartezeit-Timer für die Simulation von Ladezeiten</t>
-  </si>
-  <si>
-    <t>nuntius_printer_startWaitTime</t>
-  </si>
-  <si>
-    <t>nuntius_printer_goToPageAfterWaitTime</t>
-  </si>
-  <si>
-    <t>Öffnet die "Bitte Warten"-Seite für die Ladezeit-Simulation</t>
-  </si>
-  <si>
-    <t>Wartezeit in Sekunden</t>
-  </si>
-  <si>
-    <t>Wait-Reason für die Ladezeit</t>
-  </si>
-  <si>
-    <t>Zielseite nach Ablauf der Wartezeit</t>
-  </si>
-  <si>
-    <t>Startet die Wartezeit mit dem gegebenen Wartegrund</t>
+7 = Abmelden
+10 = Fahrerkarte nach der Pause einlesen</t>
   </si>
 </sst>
 </file>
@@ -2122,8 +2123,8 @@
   </sheetPr>
   <dimension ref="A1:B117"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2481,12 +2482,12 @@
         <v>350</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="165" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>550</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2765,10 +2766,10 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>557</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -3170,10 +3171,10 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>559</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -3642,8 +3643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717CEF75-956F-4D6D-ADE3-21264BBAF87D}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88:B110"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3930,10 +3931,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>560</v>
+      </c>
+      <c r="B32" t="s">
         <v>561</v>
-      </c>
-      <c r="B32" t="s">
-        <v>562</v>
       </c>
       <c r="C32" t="s">
         <v>251</v>
@@ -4362,30 +4363,30 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>563</v>
+      </c>
+      <c r="B81" t="s">
         <v>564</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>565</v>
       </c>
-      <c r="D81" t="s">
-        <v>566</v>
-      </c>
       <c r="E81" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B82" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D82" t="s">
+        <v>565</v>
+      </c>
+      <c r="E82" t="s">
         <v>566</v>
-      </c>
-      <c r="E82" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -4482,7 +4483,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B96" s="13"/>
       <c r="D96" s="13"/>

</xml_diff>